<commit_message>
reading and editing pdfs
</commit_message>
<xml_diff>
--- a/example2.xlsx
+++ b/example2.xlsx
@@ -7,10 +7,11 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="My other sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="My New Sheet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="My other sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="My other sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="My New Sheet" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -366,6 +367,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -391,24 +410,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -425,4 +426,22 @@
   <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>